<commit_message>
Last Commit on 17Apr2023
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/AMSTestData.xlsx
+++ b/src/main/java/com/testData/AMSTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF93E83-FF76-4C76-A05B-199BF9EFBBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72291BEB-0D40-45C5-B57C-333C848E3963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12375" yWindow="615" windowWidth="10770" windowHeight="9030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="9780" windowWidth="10770" windowHeight="9030" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="2" r:id="rId1"/>
@@ -975,9 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC224A1C-134D-4208-AE57-F4FC9B3C552F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
first commit on 14Apr2023
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/AMSTestData.xlsx
+++ b/src/main/java/com/testData/AMSTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72291BEB-0D40-45C5-B57C-333C848E3963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B01312-B7B8-4CF2-B0B8-47D587AED6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="9780" windowWidth="10770" windowHeight="9030" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6795" yWindow="1080" windowWidth="10770" windowHeight="8100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>Username</t>
   </si>
@@ -227,9 +227,6 @@
     <t>AssetNumber</t>
   </si>
   <si>
-    <t>4632301660</t>
-  </si>
-  <si>
     <t>4632301661</t>
   </si>
   <si>
@@ -260,13 +257,40 @@
     <t>CreateAssetSuccessfullMessage</t>
   </si>
   <si>
-    <t>Akash Dhole</t>
-  </si>
-  <si>
     <t>01242022</t>
   </si>
   <si>
-    <t>akash.dhole@in.ncs-i.com</t>
+    <t>4632301662</t>
+  </si>
+  <si>
+    <t>NewEmployeeId</t>
+  </si>
+  <si>
+    <t>NewEmployeeName</t>
+  </si>
+  <si>
+    <t>NewEmpStatus</t>
+  </si>
+  <si>
+    <t>NewEmpDateOfJoining</t>
+  </si>
+  <si>
+    <t>NewEmpEmailId</t>
+  </si>
+  <si>
+    <t>Satish Jha</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>satish.jha@in.ncs-i.com</t>
+  </si>
+  <si>
+    <t>Satish M</t>
+  </si>
+  <si>
+    <t>satish.mk@in.ncs-i.com</t>
   </si>
 </sst>
 </file>
@@ -772,7 +796,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +810,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -794,7 +818,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,7 +834,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -834,7 +858,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,10 +887,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +898,7 @@
         <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,7 +906,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,7 +922,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +946,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -951,10 +975,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -973,22 +997,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC224A1C-134D-4208-AE57-F4FC9B3C552F}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="5">
-        <v>1345365</v>
+      <c r="B1" s="6">
+        <v>1359335</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -996,7 +1022,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1011,8 +1037,8 @@
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>78</v>
+      <c r="B4" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1020,20 +1046,60 @@
         <v>58</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1345385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3152022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{D6DF9AF1-632D-4969-BF8E-FF5F40315B01}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{910EB955-A826-4666-8EE2-3EE7265E1897}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Last commit on 20Apr2023
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/AMSTestData.xlsx
+++ b/src/main/java/com/testData/AMSTestData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B01312-B7B8-4CF2-B0B8-47D587AED6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAEE931-98C7-41A9-B27A-27ADB5BE791E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="1080" windowWidth="10770" windowHeight="8100" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="2" r:id="rId1"/>
     <sheet name="AssetModule" sheetId="3" r:id="rId2"/>
     <sheet name="EmployeeModule" sheetId="5" r:id="rId3"/>
+    <sheet name="AssetsGroup" sheetId="6" r:id="rId4"/>
+    <sheet name="AssetDepartment" sheetId="7" r:id="rId5"/>
+    <sheet name="AssetVendor" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
   <si>
     <t>Username</t>
   </si>
@@ -209,18 +212,9 @@
     <t>DateOfJoining</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>EmployeeName</t>
-  </si>
-  <si>
-    <t>EmployeeID</t>
-  </si>
-  <si>
     <t>NewAssetNumber</t>
   </si>
   <si>
@@ -287,10 +281,61 @@
     <t>satish.jha@in.ncs-i.com</t>
   </si>
   <si>
-    <t>Satish M</t>
-  </si>
-  <si>
     <t>satish.mk@in.ncs-i.com</t>
+  </si>
+  <si>
+    <t>Office Eq (60Mth)</t>
+  </si>
+  <si>
+    <t>SerachAssetGroup</t>
+  </si>
+  <si>
+    <t>Office Eq (36Mth)</t>
+  </si>
+  <si>
+    <t>SuccessMessAfterCreate</t>
+  </si>
+  <si>
+    <t>DeleteMessAfterDel</t>
+  </si>
+  <si>
+    <t>Deleted!</t>
+  </si>
+  <si>
+    <t>UpdateSuccesMess</t>
+  </si>
+  <si>
+    <t>SerachAssetDepartmet</t>
+  </si>
+  <si>
+    <t>AssetDepartment</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>NewAssetDepartment</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Orient technologies</t>
+  </si>
+  <si>
+    <t>Dynamic Distributors</t>
+  </si>
+  <si>
+    <t>AssetVendorName</t>
+  </si>
+  <si>
+    <t>AssetVendorCode</t>
+  </si>
+  <si>
+    <t>NewAssetVendorName</t>
+  </si>
+  <si>
+    <t>NewAssetVendorCode</t>
   </si>
 </sst>
 </file>
@@ -342,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -360,6 +405,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -807,10 +855,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -818,7 +866,7 @@
         <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -834,7 +882,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,7 +906,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -887,18 +935,18 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -906,7 +954,7 @@
         <v>57</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -922,7 +970,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -946,7 +994,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -975,10 +1023,10 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,21 +1045,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC224A1C-134D-4208-AE57-F4FC9B3C552F}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="6">
         <v>1359335</v>
@@ -1019,7 +1067,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>86</v>
@@ -1027,81 +1075,322 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1345385</v>
+        <v>90</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="5">
-        <v>3152022</v>
+        <v>58</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1345385</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3152022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{910EB955-A826-4666-8EE2-3EE7265E1897}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{910EB955-A826-4666-8EE2-3EE7265E1897}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EF100A-4F9A-426B-945F-8B2FB9BB4336}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DC4D8B-D072-4FF0-A12A-1E293B1DDC7E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CB5913-AEBA-469F-8C75-E4D3FDC9E665}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="8">
+        <v>46100028</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="8">
+        <v>46100034</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last commit on 21Apr2023
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/AMSTestData.xlsx
+++ b/src/main/java/com/testData/AMSTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAE64DD-EB7F-4EA1-9027-524CD4CC9EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B367DE75-B26F-4E1E-AAF6-EF52234644F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="AssetDepartment" sheetId="7" r:id="rId5"/>
     <sheet name="AssetVendor" sheetId="8" r:id="rId6"/>
     <sheet name="AssetsStatus" sheetId="9" r:id="rId7"/>
+    <sheet name="User" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
   <si>
     <t>Username</t>
   </si>
@@ -355,6 +356,54 @@
   </si>
   <si>
     <t>Present</t>
+  </si>
+  <si>
+    <t>P1345365</t>
+  </si>
+  <si>
+    <t>AkashD</t>
+  </si>
+  <si>
+    <t>akash.dhole@in.ncs-i.com</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>akash@123</t>
+  </si>
+  <si>
+    <t>AkashDhole</t>
+  </si>
+  <si>
+    <t>akash.dhole@ncs.com.sg</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>EmpID1</t>
+  </si>
+  <si>
+    <t>UserName1</t>
+  </si>
+  <si>
+    <t>Email1</t>
+  </si>
+  <si>
+    <t>Role1</t>
+  </si>
+  <si>
+    <t>UserPassword1</t>
+  </si>
+  <si>
+    <t>NewUsername1</t>
+  </si>
+  <si>
+    <t>NewEmail1</t>
+  </si>
+  <si>
+    <t>ChangeRole1</t>
   </si>
 </sst>
 </file>
@@ -712,7 +761,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +912,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,13 +1116,13 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="42" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1409,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:B5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DAD6EBF-BE7C-453D-9F7B-18AEF0473DC9}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,4 +1506,96 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F427F976-C216-4B48-9E9C-FA96F73AF759}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Commit on 26Apr2023
</commit_message>
<xml_diff>
--- a/src/main/java/com/testData/AMSTestData.xlsx
+++ b/src/main/java/com/testData/AMSTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Projects\Selenabler_Framework\Selenabler2.0\src\main\java\com\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B367DE75-B26F-4E1E-AAF6-EF52234644F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB22788-ED5F-4AAF-9A02-838059CFE090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSheet" sheetId="2" r:id="rId1"/>
@@ -460,7 +460,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -477,6 +476,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614DE2D3-F2DC-4676-B578-354236B00B50}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +854,7 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -899,11 +899,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{5817C4B5-4D3F-44B1-9699-5C6F6BD92089}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -925,7 +922,7 @@
       <c r="A1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -933,7 +930,7 @@
       <c r="A2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -941,7 +938,7 @@
       <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -949,7 +946,7 @@
       <c r="A4" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -957,7 +954,7 @@
       <c r="A5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -965,7 +962,7 @@
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -973,7 +970,7 @@
       <c r="A7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -981,7 +978,7 @@
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -989,7 +986,7 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -997,7 +994,7 @@
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1005,7 +1002,7 @@
       <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1013,7 +1010,7 @@
       <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1021,7 +1018,7 @@
       <c r="A13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1029,7 +1026,7 @@
       <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1037,7 +1034,7 @@
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1045,7 +1042,7 @@
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1053,7 +1050,7 @@
       <c r="A17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1061,7 +1058,7 @@
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1069,7 +1066,7 @@
       <c r="A19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1077,7 +1074,7 @@
       <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1085,7 +1082,7 @@
       <c r="A21" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1093,7 +1090,7 @@
       <c r="A22" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1101,7 +1098,7 @@
       <c r="A23" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1122,126 +1119,126 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="42" style="5" customWidth="1"/>
+    <col min="2" max="2" width="42" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="6">
+      <c r="B1" s="5">
         <v>1359335</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>1345385</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>3152022</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1415,15 +1412,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1431,7 +1428,7 @@
       <c r="A2" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1439,7 +1436,7 @@
       <c r="A3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1447,7 +1444,7 @@
       <c r="A4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1455,7 +1452,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1483,7 +1480,7 @@
       <c r="A1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1491,7 +1488,7 @@
       <c r="A2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1499,7 +1496,7 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1512,21 +1509,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F427F976-C216-4B48-9E9C-FA96F73AF759}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1534,7 +1531,7 @@
       <c r="A2" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1542,7 +1539,7 @@
       <c r="A3" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1550,7 +1547,7 @@
       <c r="A4" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1558,7 +1555,7 @@
       <c r="A5" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1566,7 +1563,7 @@
       <c r="A6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1574,7 +1571,7 @@
       <c r="A7" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1582,7 +1579,7 @@
       <c r="A8" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1590,7 +1587,7 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>